<commit_message>
added revision of bosl board
</commit_message>
<xml_diff>
--- a/Board-Hardware/Manufacturing/BoSL BOM Rev 0.4.xlsx
+++ b/Board-Hardware/Manufacturing/BoSL BOM Rev 0.4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Monash-BoSL\Board-Hardware\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB52793-B39D-4105-9F08-0B189F188DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B347CF-97B1-4834-A76A-238871A8AA66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
   <si>
     <t>Part Number</t>
   </si>
@@ -459,6 +459,30 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/product-detail/en/microchip-technology/ATMEGA328P-AUR/ATMEGA328P-AURCT-ND/3789455</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/keystone-electronics/2996TR/36-2996CT-ND/5878110</t>
+  </si>
+  <si>
+    <t>Battery Clip</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>2996TR</t>
+  </si>
+  <si>
+    <t>Button Cell Battery</t>
+  </si>
+  <si>
+    <t>LR44</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/murata-electronics/LR44/490-18190-ND/9859017</t>
+  </si>
+  <si>
+    <t>1.5 V</t>
   </si>
 </sst>
 </file>
@@ -875,7 +899,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1744,7 +1768,7 @@
         <v>3.77</v>
       </c>
       <c r="H32" s="18">
-        <f>G32*F32</f>
+        <f t="shared" ref="H32:H39" si="1">G32*F32</f>
         <v>3.77</v>
       </c>
       <c r="I32" s="3" t="s">
@@ -1765,7 +1789,7 @@
         <v>1.98</v>
       </c>
       <c r="H33" s="18">
-        <f>G33*F33</f>
+        <f t="shared" si="1"/>
         <v>1.98</v>
       </c>
       <c r="I33" s="3" t="s">
@@ -1792,7 +1816,7 @@
         <v>0.1</v>
       </c>
       <c r="H34" s="18">
-        <f>G34*F34</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
@@ -1819,7 +1843,7 @@
         <v>0.1</v>
       </c>
       <c r="H35" s="15">
-        <f>G35*F35</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="I35" s="3"/>
@@ -1841,7 +1865,7 @@
         <v>0.77</v>
       </c>
       <c r="H36" s="15">
-        <f>G36*F36</f>
+        <f t="shared" si="1"/>
         <v>0.77</v>
       </c>
       <c r="I36" s="3" t="s">
@@ -1869,7 +1893,7 @@
         <v>0.43</v>
       </c>
       <c r="H37" s="15">
-        <f>G37*F37</f>
+        <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
       <c r="I37" s="3" t="s">
@@ -1877,12 +1901,53 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="G38" s="17"/>
-      <c r="I38" s="3"/>
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="15">
+        <v>0.63</v>
+      </c>
+      <c r="H38" s="15">
+        <f t="shared" si="1"/>
+        <v>0.63</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="G39" s="17"/>
-      <c r="I39" s="3"/>
+      <c r="A39" s="17"/>
+      <c r="B39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H39" s="15">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
       <c r="G40" s="17"/>

</xml_diff>

<commit_message>
added space savings of BoSL PCB
</commit_message>
<xml_diff>
--- a/Board-Hardware/Manufacturing/BoSL BOM Rev 0.4.xlsx
+++ b/Board-Hardware/Manufacturing/BoSL BOM Rev 0.4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20356"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Monash-BoSL\Board-Hardware\Manufacturing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Monash-BoSL\Board-Hardware\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B347CF-97B1-4834-A76A-238871A8AA66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725048B5-A323-4C7A-B159-31C76A0937DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="152">
   <si>
     <t>Part Number</t>
   </si>
@@ -266,12 +256,6 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>Through Hole</t>
-  </si>
-  <si>
-    <t>https://www.altronics.com.au/p/v1249a-8.000000mhz-low-profile-hc49s-crystal/</t>
-  </si>
-  <si>
     <t xml:space="preserve">3-Pin SOT-89 </t>
   </si>
   <si>
@@ -483,6 +467,15 @@
   </si>
   <si>
     <t>1.5 V</t>
+  </si>
+  <si>
+    <t>2-SMD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ecs-inc/ECS-80-18-30-JGN-TR/XC2103CT-ND/5875587</t>
+  </si>
+  <si>
+    <t>ECS-80-18-30-JGN-TR</t>
   </si>
 </sst>
 </file>
@@ -492,7 +485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +566,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -596,7 +595,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -619,6 +618,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -921,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -930,13 +930,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -950,7 +950,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -994,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1019,7 +1019,7 @@
         <v>1.5</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1054,10 +1054,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1076,7 +1076,7 @@
         <v>0.6</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1112,7 +1112,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -1160,16 +1160,16 @@
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1216,7 +1216,7 @@
         <v>33</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
@@ -1244,7 +1244,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -1275,7 +1275,7 @@
         <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -1302,10 +1302,10 @@
         <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -1330,10 +1330,10 @@
         <v>33</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
         <v>44</v>
@@ -1358,7 +1358,7 @@
         <v>33</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -1411,7 +1411,7 @@
         <v>33</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
         <v>50</v>
@@ -1439,7 +1439,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>53</v>
@@ -1467,7 +1467,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
         <v>55</v>
@@ -1495,7 +1495,7 @@
         <v>33</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
         <v>57</v>
@@ -1574,10 +1574,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>78</v>
+        <v>151</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>149</v>
       </c>
       <c r="C25" t="s">
         <v>66</v>
@@ -1592,26 +1592,26 @@
         <v>1</v>
       </c>
       <c r="G25" s="15">
-        <v>0.1</v>
+        <v>0.69</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.69</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
         <v>84</v>
-      </c>
-      <c r="D26" t="s">
-        <v>86</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1624,21 +1624,21 @@
         <v>19</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1651,21 +1651,21 @@
         <v>1.5</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1678,21 +1678,21 @@
         <v>0.75</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1705,19 +1705,19 @@
         <v>2.16</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1730,22 +1730,22 @@
         <v>2.5</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1"/>
       <c r="B31" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" t="s">
         <v>110</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" t="s">
-        <v>112</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -1753,13 +1753,13 @@
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1">
       <c r="A32" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1772,15 +1772,15 @@
         <v>3.77</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="3" customFormat="1">
       <c r="A33" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
@@ -1793,7 +1793,7 @@
         <v>1.98</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="3" customFormat="1">
@@ -1801,13 +1801,13 @@
         <v>33</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
@@ -1825,16 +1825,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F35" s="3">
         <v>2</v>
@@ -1850,13 +1850,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
@@ -1869,22 +1869,22 @@
         <v>0.77</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
@@ -1897,18 +1897,18 @@
         <v>0.43</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
@@ -1921,19 +1921,19 @@
         <v>0.63</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="17"/>
       <c r="B39" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" t="s">
         <v>148</v>
-      </c>
-      <c r="D39" t="s">
-        <v>147</v>
-      </c>
-      <c r="E39" t="s">
-        <v>150</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
@@ -1946,7 +1946,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1963,17 +1963,16 @@
     <hyperlink ref="I8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="I4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="I5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="I25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I26" r:id="rId10" display="https://www.aliexpress.com/item/32963816626.html?spm=2114.search0604.3.36.61e15ac4BS3gJ9&amp;ws_ab_test=searchweb0_0%2Csearchweb201602_6_10065_10130_10068_10547_319_317_10548_10696_453_10084_454_10083_10618_10307_537_536_10131_10132_10133_10059_10884_10887_321_322_10103%2Csearchweb201603_51%2CppcSwitch_0&amp;algo_expid=a8ad79e3-3036-4b7a-8391-3f73e7497cac-5&amp;algo_pvid=a8ad79e3-3036-4b7a-8391-3f73e7497cac" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="I27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="I28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="I30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="I3" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="I6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="I10" r:id="rId16" xr:uid="{68617DBC-81B6-4EF9-9C99-38891EFD4A08}"/>
-    <hyperlink ref="I7" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I26" r:id="rId9" display="https://www.aliexpress.com/item/32963816626.html?spm=2114.search0604.3.36.61e15ac4BS3gJ9&amp;ws_ab_test=searchweb0_0%2Csearchweb201602_6_10065_10130_10068_10547_319_317_10548_10696_453_10084_454_10083_10618_10307_537_536_10131_10132_10133_10059_10884_10887_321_322_10103%2Csearchweb201603_51%2CppcSwitch_0&amp;algo_expid=a8ad79e3-3036-4b7a-8391-3f73e7497cac-5&amp;algo_pvid=a8ad79e3-3036-4b7a-8391-3f73e7497cac" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I27" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I28" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I30" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I3" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I10" r:id="rId15" xr:uid="{68617DBC-81B6-4EF9-9C99-38891EFD4A08}"/>
+    <hyperlink ref="I7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed velocity  code to get 3 attempts to get amplitude > 1000
</commit_message>
<xml_diff>
--- a/Board-Hardware/Manufacturing/BoSL BOM Rev 0.4.xlsx
+++ b/Board-Hardware/Manufacturing/BoSL BOM Rev 0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Monash-BoSL\Board-Hardware\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9326E202-A145-4CB8-850D-7ABD3533591C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D183A6-2782-4298-88C9-A2F6E31A5EDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -892,7 +892,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>